<commit_message>
Updating Data Dictionary with Essential column
</commit_message>
<xml_diff>
--- a/dd/GoTechnology_hub2_DataDictionary.xlsx
+++ b/dd/GoTechnology_hub2_DataDictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://woodplc-my.sharepoint.com/personal/josh_goolnik_woodplc_com/Documents/hub2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GoTechnology\GoTechnology.github.io\dd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="447" documentId="8_{3A0BE2BA-C9DB-4C69-A21C-B0A66D4A1041}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{6A7E1E3F-2352-4906-B77D-61B4AA99FA3B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F313B50A-A102-4E2B-8261-5A577A08C0E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{1FA7F18E-DDF7-462D-97AC-5A5AC7B89923}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1FA7F18E-DDF7-462D-97AC-5A5AC7B89923}"/>
   </bookViews>
   <sheets>
     <sheet name="DataDictionary" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="173">
   <si>
     <t>Table</t>
   </si>
@@ -647,6 +647,15 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>Essential</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -760,12 +769,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -776,11 +779,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
     <dxf>
       <font>
         <strike val="0"/>
@@ -806,6 +815,23 @@
         <color theme="1"/>
         <name val="Segoe UI"/>
         <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -909,6 +935,16 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -923,18 +959,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4944ACD-47D7-404C-8A19-08F9A36D7F75}" name="Table1" displayName="Table1" ref="A3:H65" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A3:H65" xr:uid="{C51D7F9D-8A9E-4710-9A57-2EACFF5E232B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4944ACD-47D7-404C-8A19-08F9A36D7F75}" name="Table1" displayName="Table1" ref="A3:I65" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A3:I65" xr:uid="{C51D7F9D-8A9E-4710-9A57-2EACFF5E232B}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="B"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I65">
     <sortCondition ref="F3:F65"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{92122F83-691A-4EFD-B566-570A2A3CA0D9}" name="Table"/>
-    <tableColumn id="2" xr3:uid="{195E4C95-5432-4C16-9278-9034FDE79B51}" name="Definition" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{D3FFE813-801A-4BFC-A892-721987F58731}" name="Example Values" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{5254EBA8-3EA6-4853-A011-5969412F4970}" name="Menu Location" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{02EA6424-1CD9-4F54-9401-A47E8CA78072}" name="Level" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{B66D16DE-8CC4-41D5-8309-485740CB6557}" name="Load Order" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{195E4C95-5432-4C16-9278-9034FDE79B51}" name="Definition" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{D3FFE813-801A-4BFC-A892-721987F58731}" name="Example Values" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{5254EBA8-3EA6-4853-A011-5969412F4970}" name="Menu Location" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{02EA6424-1CD9-4F54-9401-A47E8CA78072}" name="Level" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{B66D16DE-8CC4-41D5-8309-485740CB6557}" name="Load Order" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{9AB8566A-A4A5-4E93-BBB1-9DBD150A7BD0}" name="Essential" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{FEF00463-B75D-4529-AA2B-58BC157D606E}" name="References" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{EA900B4D-8397-4512-8CA2-2E5FF59DEA09}" name="Referenced By" dataDxfId="0"/>
   </tableColumns>
@@ -1239,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46346F6C-6515-44A2-AC18-B26BE2AACDE3}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1252,37 +1295,39 @@
     <col min="3" max="3" width="41.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="7" width="12.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1302,37 +1347,43 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="11">
         <v>1</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="G4" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>144</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1347,11 +1398,14 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="G5" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="264" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="264" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1370,11 +1424,14 @@
       <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="G6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -1393,11 +1450,14 @@
       <c r="F7" s="1">
         <v>4</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -1416,11 +1476,14 @@
       <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="G8" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>123</v>
       </c>
@@ -1436,11 +1499,14 @@
       <c r="F9" s="1">
         <v>6</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>118</v>
       </c>
@@ -1453,15 +1519,18 @@
       <c r="F10" s="1">
         <v>7</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>141</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1473,11 +1542,14 @@
       <c r="F11" s="1">
         <v>8</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -1493,11 +1565,14 @@
       <c r="F12" s="1">
         <v>9</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="G12" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="99" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="99" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -1516,11 +1591,14 @@
       <c r="F13" s="1">
         <v>10</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -1533,11 +1611,14 @@
       <c r="F14" s="1">
         <v>11</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="G14" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="264" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="264" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -1556,11 +1637,14 @@
       <c r="F15" s="1">
         <v>12</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="G15" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="165" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>126</v>
       </c>
@@ -1576,11 +1660,14 @@
       <c r="F16" s="1">
         <v>13</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="G16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>125</v>
       </c>
@@ -1596,8 +1683,11 @@
       <c r="F17" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="G17" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -1613,11 +1703,14 @@
       <c r="F18" s="1">
         <v>15</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="G18" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -1633,11 +1726,14 @@
       <c r="F19" s="1">
         <v>16</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="G19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="280.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="280.5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -1653,11 +1749,14 @@
       <c r="F20" s="1">
         <v>17</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="G20" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>119</v>
       </c>
@@ -1673,12 +1772,15 @@
       <c r="F21" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G21" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>132</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1690,8 +1792,11 @@
       <c r="F22" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="G22" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -1707,8 +1812,11 @@
       <c r="F23" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="G23" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -1724,8 +1832,11 @@
       <c r="F24" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G24" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>121</v>
       </c>
@@ -1744,8 +1855,11 @@
       <c r="F25" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G25" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -1761,8 +1875,11 @@
       <c r="F26" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="G26" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="66" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1778,11 +1895,14 @@
       <c r="F27" s="1">
         <v>24</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="G27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1798,11 +1918,14 @@
       <c r="F28" s="1">
         <v>25</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="G28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="132" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1818,11 +1941,14 @@
       <c r="F29" s="1">
         <v>26</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="G29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="132" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1838,11 +1964,14 @@
       <c r="F30" s="1">
         <v>27</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="G30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1858,11 +1987,14 @@
       <c r="F31" s="1">
         <v>28</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="G31" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1878,15 +2010,18 @@
       <c r="F32" s="1">
         <v>29</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="G32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="8" t="s">
         <v>70</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -1898,11 +2033,14 @@
       <c r="F33" s="1">
         <v>30</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="G33" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1918,11 +2056,14 @@
       <c r="F34" s="1">
         <v>31</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="G34" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="264" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="264" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1938,11 +2079,14 @@
       <c r="F35" s="1">
         <v>32</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="G35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1958,11 +2102,14 @@
       <c r="F36" s="1">
         <v>33</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="G36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="181.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -1978,11 +2125,14 @@
       <c r="F37" s="1">
         <v>34</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="G37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="409.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -1998,11 +2148,14 @@
       <c r="F38" s="1">
         <v>35</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="G38" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -2018,11 +2171,14 @@
       <c r="F39" s="1">
         <v>36</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="G39" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="99" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="99" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -2038,11 +2194,14 @@
       <c r="F40" s="1">
         <v>37</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="G40" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -2058,8 +2217,11 @@
       <c r="F41" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="G41" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="115.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>158</v>
       </c>
@@ -2075,11 +2237,14 @@
       <c r="F42" s="1">
         <v>39</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="G42" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I42" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -2095,11 +2260,14 @@
       <c r="F43" s="1">
         <v>40</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="G43" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="198" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="198" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2115,11 +2283,14 @@
       <c r="F44" s="1">
         <v>41</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="G44" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -2135,8 +2306,11 @@
       <c r="F45" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="G45" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -2152,11 +2326,14 @@
       <c r="F46" s="1">
         <v>43</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="G46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I46" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="49.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -2172,8 +2349,11 @@
       <c r="F47" s="1">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="G47" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="66" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -2189,11 +2369,14 @@
       <c r="F48" s="1">
         <v>45</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="G48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="99" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="99" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -2209,8 +2392,11 @@
       <c r="F49" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+      <c r="G49" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="132" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -2226,8 +2412,11 @@
       <c r="F50" s="1">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="132" x14ac:dyDescent="0.3">
+      <c r="G50" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="132" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -2243,8 +2432,11 @@
       <c r="F51" s="1">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="297" x14ac:dyDescent="0.3">
+      <c r="G51" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="297" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -2260,8 +2452,11 @@
       <c r="F52" s="1">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="165" x14ac:dyDescent="0.3">
+      <c r="G52" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -2277,11 +2472,14 @@
       <c r="F53" s="1">
         <v>50</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="G53" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="115.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>21</v>
       </c>
@@ -2297,11 +2495,14 @@
       <c r="F54" s="1">
         <v>51</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="G54" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="198" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="198" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -2317,8 +2518,11 @@
       <c r="F55" s="1">
         <v>52</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="99" x14ac:dyDescent="0.3">
+      <c r="G55" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="99" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -2334,11 +2538,14 @@
       <c r="F56" s="1">
         <v>53</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="G56" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I56" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="82.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>47</v>
       </c>
@@ -2354,8 +2561,11 @@
       <c r="F57" s="1">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G57" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2371,8 +2581,11 @@
       <c r="F58" s="1">
         <v>55</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="G58" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="409.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -2388,8 +2601,11 @@
       <c r="F59" s="1">
         <v>56</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="G59" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="66" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -2405,8 +2621,11 @@
       <c r="F60" s="1">
         <v>57</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="280.5" x14ac:dyDescent="0.3">
+      <c r="G60" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="280.5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -2422,8 +2641,11 @@
       <c r="F61" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="G61" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="66" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -2439,8 +2661,11 @@
       <c r="F62" s="1">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="G62" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="66" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>28</v>
       </c>
@@ -2456,8 +2681,11 @@
       <c r="F63" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="G63" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -2473,11 +2701,14 @@
       <c r="F64" s="1">
         <v>61</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="G64" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I64" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -2490,12 +2721,20 @@
       <c r="E65" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G65" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
+  <conditionalFormatting sqref="G4:G65">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",G4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Updating scripts and changing version notes structure for consistency
</commit_message>
<xml_diff>
--- a/dd/GoTechnology_hub2_DataDictionary.xlsx
+++ b/dd/GoTechnology_hub2_DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GoTechnology\GoTechnology.github.io\dd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F313B50A-A102-4E2B-8261-5A577A08C0E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DE1767-2769-4603-9670-F93441FB0EA6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1FA7F18E-DDF7-462D-97AC-5A5AC7B89923}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{1FA7F18E-DDF7-462D-97AC-5A5AC7B89923}"/>
   </bookViews>
   <sheets>
     <sheet name="DataDictionary" sheetId="1" r:id="rId1"/>
@@ -1284,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46346F6C-6515-44A2-AC18-B26BE2AACDE3}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1733,7 +1733,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="280.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="264" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -2997,15 +2997,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <MigrationWizIdPermissions xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
@@ -3015,6 +3006,15 @@
     <MigrationWizIdPermissionLevels xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3037,14 +3037,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91BF9293-7B60-4F83-9196-3CF7B73475CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F707AC79-A0C7-4998-BF58-A76D8018E1DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3059,4 +3051,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91BF9293-7B60-4F83-9196-3CF7B73475CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating data dictionary to add Work Pack Type and expand MOC Type description
</commit_message>
<xml_diff>
--- a/dd/GoTechnology_hub2_DataDictionary.xlsx
+++ b/dd/GoTechnology_hub2_DataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GoTechnology\GoTechnology.github.io\dd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870E708A-2592-4181-82A3-C06A91FD723C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84D15B6-B1F0-4B99-8BEB-73ED55696835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1FA7F18E-DDF7-462D-97AC-5A5AC7B89923}"/>
   </bookViews>
@@ -30,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="177">
   <si>
     <t>Table</t>
   </si>
@@ -278,9 +280,6 @@
   </si>
   <si>
     <t>Work Pack</t>
-  </si>
-  <si>
-    <t>The category to which the MOC item belongs: Common examples are TQ ("Technical Query") and EQ ("Engineering Query") amongst others.</t>
   </si>
   <si>
     <t xml:space="preserve">Activity within hub2 represents Level 3 in the recommended Work Breakdown Structure and as such exists as the “parent” of Job Cards and as a “child” of Level E.
@@ -656,6 +655,21 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Work Pack Type</t>
+  </si>
+  <si>
+    <t>CWP,EWP,Tier 1, Tier 2, CWP Tier 1, EWP Tier 5</t>
+  </si>
+  <si>
+    <t>EQ, TQ, GF</t>
+  </si>
+  <si>
+    <t>The category to which the Work Pack belongs. This could represent different purposes/authorisation levels/methodologies or any other type of grouping. Each Work Pack Type has it's own digital document and cover sheet, allowing a custom layout per type.</t>
+  </si>
+  <si>
+    <t>The category to which the MOC item belongs: Common examples are TQ ("Technical Query") and EQ ("Engineering Query") amongst others. Each Work Pack Type has it's own digital document and cover sheet, allowing a custom layout per type.</t>
   </si>
 </sst>
 </file>
@@ -750,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -779,6 +793,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -959,10 +976,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4944ACD-47D7-404C-8A19-08F9A36D7F75}" name="Table1" displayName="Table1" ref="A3:I65" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A3:I65" xr:uid="{C51D7F9D-8A9E-4710-9A57-2EACFF5E232B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I65">
-    <sortCondition ref="F3:F65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4944ACD-47D7-404C-8A19-08F9A36D7F75}" name="Table1" displayName="Table1" ref="A3:I66" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A3:I66" xr:uid="{C51D7F9D-8A9E-4710-9A57-2EACFF5E232B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I66">
+    <sortCondition ref="F3:F66"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{92122F83-691A-4EFD-B566-570A2A3CA0D9}" name="Table"/>
@@ -1276,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46346F6C-6515-44A2-AC18-B26BE2AACDE3}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1296,30 +1313,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="A1" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="A2" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1329,7 +1346,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -1341,25 +1358,25 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>168</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>169</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>10</v>
@@ -1368,20 +1385,20 @@
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
@@ -1393,10 +1410,10 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="264" x14ac:dyDescent="0.3">
@@ -1404,10 +1421,10 @@
         <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
@@ -1419,21 +1436,21 @@
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>18</v>
@@ -1445,21 +1462,21 @@
         <v>4</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>18</v>
@@ -1471,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>30</v>
@@ -1479,10 +1496,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>18</v>
@@ -1494,15 +1511,15 @@
         <v>6</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>18</v>
@@ -1514,18 +1531,18 @@
         <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>18</v>
@@ -1537,7 +1554,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>57</v>
@@ -1545,10 +1562,10 @@
     </row>
     <row r="12" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>18</v>
@@ -1560,7 +1577,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>57</v>
@@ -1568,13 +1585,13 @@
     </row>
     <row r="13" spans="1:9" ht="99" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>18</v>
@@ -1586,7 +1603,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>66</v>
@@ -1594,7 +1611,7 @@
     </row>
     <row r="14" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>18</v>
@@ -1606,21 +1623,21 @@
         <v>11</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="264" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>18</v>
@@ -1632,7 +1649,7 @@
         <v>12</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>73</v>
@@ -1640,10 +1657,10 @@
     </row>
     <row r="16" spans="1:9" ht="165" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
@@ -1655,18 +1672,18 @@
         <v>13</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>18</v>
@@ -1678,15 +1695,15 @@
         <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>18</v>
@@ -1698,18 +1715,18 @@
         <v>15</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>18</v>
@@ -1721,18 +1738,18 @@
         <v>16</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="264" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="280.5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>18</v>
@@ -1744,7 +1761,7 @@
         <v>17</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>75</v>
@@ -1752,10 +1769,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>18</v>
@@ -1767,15 +1784,15 @@
         <v>18</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>18</v>
@@ -1787,15 +1804,15 @@
         <v>19</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>18</v>
@@ -1807,15 +1824,15 @@
         <v>20</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>18</v>
@@ -1827,18 +1844,18 @@
         <v>21</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>18</v>
@@ -1850,15 +1867,15 @@
         <v>22</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>18</v>
@@ -1870,7 +1887,7 @@
         <v>23</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="66" x14ac:dyDescent="0.3">
@@ -1890,10 +1907,10 @@
         <v>24</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
@@ -1913,10 +1930,10 @@
         <v>25</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="132" x14ac:dyDescent="0.3">
@@ -1936,10 +1953,10 @@
         <v>26</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="132" x14ac:dyDescent="0.3">
@@ -1959,10 +1976,10 @@
         <v>27</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
@@ -1982,10 +1999,10 @@
         <v>28</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
@@ -1993,7 +2010,7 @@
         <v>71</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>18</v>
@@ -2005,10 +2022,10 @@
         <v>29</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="165" x14ac:dyDescent="0.3">
@@ -2028,10 +2045,10 @@
         <v>30</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
@@ -2051,10 +2068,10 @@
         <v>31</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="264" x14ac:dyDescent="0.3">
@@ -2074,18 +2091,21 @@
         <v>32</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>44</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>80</v>
+        <v>176</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>18</v>
@@ -2097,7 +2117,7 @@
         <v>33</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>42</v>
@@ -2108,7 +2128,7 @@
         <v>50</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>18</v>
@@ -2120,7 +2140,7 @@
         <v>34</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>47</v>
@@ -2131,7 +2151,7 @@
         <v>30</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>18</v>
@@ -2143,7 +2163,7 @@
         <v>35</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>73</v>
@@ -2154,7 +2174,7 @@
         <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>18</v>
@@ -2166,7 +2186,7 @@
         <v>36</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>75</v>
@@ -2177,7 +2197,7 @@
         <v>25</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>18</v>
@@ -2189,7 +2209,7 @@
         <v>37</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>26</v>
@@ -2212,15 +2232,15 @@
         <v>38</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>18</v>
@@ -2232,10 +2252,10 @@
         <v>39</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
@@ -2255,10 +2275,10 @@
         <v>40</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="198" x14ac:dyDescent="0.3">
@@ -2266,7 +2286,7 @@
         <v>72</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>20</v>
@@ -2278,7 +2298,7 @@
         <v>41</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>73</v>
@@ -2301,7 +2321,7 @@
         <v>42</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
@@ -2321,10 +2341,10 @@
         <v>43</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
@@ -2344,7 +2364,7 @@
         <v>44</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="66" x14ac:dyDescent="0.3">
@@ -2364,7 +2384,7 @@
         <v>45</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>40</v>
@@ -2375,7 +2395,7 @@
         <v>68</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>20</v>
@@ -2387,7 +2407,7 @@
         <v>46</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="132" x14ac:dyDescent="0.3">
@@ -2407,7 +2427,7 @@
         <v>47</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="132" x14ac:dyDescent="0.3">
@@ -2415,7 +2435,7 @@
         <v>19</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>20</v>
@@ -2427,7 +2447,7 @@
         <v>48</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="297" x14ac:dyDescent="0.3">
@@ -2435,7 +2455,7 @@
         <v>42</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>43</v>
@@ -2447,7 +2467,7 @@
         <v>49</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="165" x14ac:dyDescent="0.3">
@@ -2455,7 +2475,7 @@
         <v>5</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>6</v>
@@ -2467,7 +2487,7 @@
         <v>50</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>31</v>
@@ -2490,38 +2510,45 @@
         <v>51</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="198" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="55" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A55" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="11">
+        <v>52</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F55" s="1">
-        <v>52</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="99" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:9" ht="198" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>18</v>
@@ -2533,21 +2560,18 @@
         <v>53</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="99" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>7</v>
@@ -2556,18 +2580,21 @@
         <v>54</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>7</v>
@@ -2576,15 +2603,15 @@
         <v>55</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>64</v>
@@ -2596,18 +2623,18 @@
         <v>56</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>7</v>
@@ -2616,18 +2643,18 @@
         <v>57</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="280.5" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>7</v>
@@ -2636,18 +2663,18 @@
         <v>58</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="280.5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>7</v>
@@ -2656,18 +2683,18 @@
         <v>59</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>7</v>
@@ -2676,18 +2703,18 @@
         <v>60</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>7</v>
@@ -2696,27 +2723,50 @@
         <v>61</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I64" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="1">
+        <v>61</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G65" s="1" t="s">
-        <v>172</v>
+      <c r="F66" s="1">
+        <v>62</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2724,7 +2774,7 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G4:G65">
+  <conditionalFormatting sqref="G4:G66">
     <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",G4)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updating data dictionary to include Professions
</commit_message>
<xml_diff>
--- a/dd/GoTechnology_hub2_DataDictionary.xlsx
+++ b/dd/GoTechnology_hub2_DataDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GoTechnology\GoTechnology.github.io\dd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84D15B6-B1F0-4B99-8BEB-73ED55696835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A822889-78C1-4287-9135-3F72AA72E2E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1FA7F18E-DDF7-462D-97AC-5A5AC7B89923}"/>
   </bookViews>
@@ -17,10 +17,10 @@
     <sheet name="About" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_ftn1" localSheetId="0">DataDictionary!$A$94</definedName>
-    <definedName name="_ftnref1" localSheetId="0">DataDictionary!$B$77</definedName>
+    <definedName name="_ftn1" localSheetId="0">DataDictionary!$A$95</definedName>
+    <definedName name="_ftnref1" localSheetId="0">DataDictionary!$B$78</definedName>
     <definedName name="_Hlk512869487" localSheetId="0">DataDictionary!$B$9</definedName>
-    <definedName name="_Hlk512870131" localSheetId="0">DataDictionary!$A$58</definedName>
+    <definedName name="_Hlk512870131" localSheetId="0">DataDictionary!$A$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="181">
   <si>
     <t>Table</t>
   </si>
@@ -670,6 +670,19 @@
   </si>
   <si>
     <t>The category to which the MOC item belongs: Common examples are TQ ("Technical Query") and EQ ("Engineering Query") amongst others. Each Work Pack Type has it's own digital document and cover sheet, allowing a custom layout per type.</t>
+  </si>
+  <si>
+    <t>Profession</t>
+  </si>
+  <si>
+    <t>A grouping of Authorised Persons and Disciplines, alllows definition of who is responsible for what discipline scopes.</t>
+  </si>
+  <si>
+    <t>Electrical Technician, Piping Engineer</t>
+  </si>
+  <si>
+    <t>Authorised Person
+Discipline</t>
   </si>
 </sst>
 </file>
@@ -764,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -802,11 +815,24 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -952,16 +978,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -976,21 +992,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4944ACD-47D7-404C-8A19-08F9A36D7F75}" name="Table1" displayName="Table1" ref="A3:I66" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A3:I66" xr:uid="{C51D7F9D-8A9E-4710-9A57-2EACFF5E232B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I66">
-    <sortCondition ref="F3:F66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4944ACD-47D7-404C-8A19-08F9A36D7F75}" name="Table1" displayName="Table1" ref="A3:I67" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A3:I67" xr:uid="{C51D7F9D-8A9E-4710-9A57-2EACFF5E232B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I67">
+    <sortCondition ref="F3:F67"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{92122F83-691A-4EFD-B566-570A2A3CA0D9}" name="Table"/>
-    <tableColumn id="2" xr3:uid="{195E4C95-5432-4C16-9278-9034FDE79B51}" name="Definition" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{D3FFE813-801A-4BFC-A892-721987F58731}" name="Example Values" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{5254EBA8-3EA6-4853-A011-5969412F4970}" name="Menu Location" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{02EA6424-1CD9-4F54-9401-A47E8CA78072}" name="Level" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{B66D16DE-8CC4-41D5-8309-485740CB6557}" name="Load Order" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{9AB8566A-A4A5-4E93-BBB1-9DBD150A7BD0}" name="Essential" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{FEF00463-B75D-4529-AA2B-58BC157D606E}" name="References" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{EA900B4D-8397-4512-8CA2-2E5FF59DEA09}" name="Referenced By" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{195E4C95-5432-4C16-9278-9034FDE79B51}" name="Definition" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{D3FFE813-801A-4BFC-A892-721987F58731}" name="Example Values" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{5254EBA8-3EA6-4853-A011-5969412F4970}" name="Menu Location" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{02EA6424-1CD9-4F54-9401-A47E8CA78072}" name="Level" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{B66D16DE-8CC4-41D5-8309-485740CB6557}" name="Load Order" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{9AB8566A-A4A5-4E93-BBB1-9DBD150A7BD0}" name="Essential" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{FEF00463-B75D-4529-AA2B-58BC157D606E}" name="References" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{EA900B4D-8397-4512-8CA2-2E5FF59DEA09}" name="Referenced By" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1293,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46346F6C-6515-44A2-AC18-B26BE2AACDE3}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29:F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1433,7 +1449,7 @@
         <v>24</v>
       </c>
       <c r="F6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>170</v>
@@ -1744,7 +1760,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="280.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="264" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -2097,15 +2113,15 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="264" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>179</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>18</v>
@@ -2117,18 +2133,24 @@
         <v>33</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="165" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>92</v>
+        <v>176</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>18</v>
@@ -2143,15 +2165,15 @@
         <v>171</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="165" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>18</v>
@@ -2163,18 +2185,18 @@
         <v>35</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>18</v>
@@ -2186,18 +2208,18 @@
         <v>36</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="99" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>18</v>
@@ -2209,18 +2231,18 @@
         <v>37</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="99" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>18</v>
@@ -2234,13 +2256,16 @@
       <c r="G41" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="I41" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>157</v>
+        <v>26</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>18</v>
@@ -2254,16 +2279,13 @@
       <c r="G42" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>18</v>
@@ -2275,21 +2297,21 @@
         <v>40</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="198" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>10</v>
@@ -2298,21 +2320,21 @@
         <v>41</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="198" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>10</v>
@@ -2321,15 +2343,18 @@
         <v>42</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>59</v>
@@ -2343,16 +2368,13 @@
       <c r="G46" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="47" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>59</v>
@@ -2366,16 +2388,19 @@
       <c r="G47" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+      <c r="I47" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>10</v>
@@ -2386,19 +2411,16 @@
       <c r="G48" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="99" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>10</v>
@@ -2409,13 +2431,16 @@
       <c r="G49" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="132" x14ac:dyDescent="0.3">
+      <c r="I49" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="99" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>20</v>
@@ -2432,10 +2457,10 @@
     </row>
     <row r="51" spans="1:9" ht="132" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>20</v>
@@ -2450,15 +2475,15 @@
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="297" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="132" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>10</v>
@@ -2470,18 +2495,18 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="165" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="297" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F53" s="1">
         <v>50</v>
@@ -2489,19 +2514,16 @@
       <c r="G53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I53" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:9" ht="165" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>7</v>
@@ -2513,48 +2535,47 @@
         <v>171</v>
       </c>
       <c r="I54" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="1">
+        <v>52</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A55" s="12" t="s">
+    <row r="56" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A56" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B56" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C56" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="D55" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="11" t="s">
+      <c r="D56" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="F55" s="11">
-        <v>52</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="198" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>79</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="F56" s="1">
         <v>53</v>
@@ -2562,13 +2583,17 @@
       <c r="G56" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="99" x14ac:dyDescent="0.3">
+      <c r="H56" s="11"/>
+      <c r="I56" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="198" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>18</v>
@@ -2582,19 +2607,16 @@
       <c r="G57" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I57" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:9" ht="99" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>7</v>
@@ -2605,16 +2627,19 @@
       <c r="G58" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I58" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>7</v>
@@ -2626,12 +2651,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>64</v>
@@ -2646,15 +2671,15 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>7</v>
@@ -2666,15 +2691,15 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="280.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>7</v>
@@ -2686,15 +2711,15 @@
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="280.5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>7</v>
@@ -2708,13 +2733,13 @@
     </row>
     <row r="64" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>7</v>
@@ -2726,46 +2751,66 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F65" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I65" s="1" t="s">
+    </row>
+    <row r="66" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="1">
+        <v>63</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>14</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F66" s="1">
-        <v>62</v>
-      </c>
-      <c r="G66" s="1" t="s">
+      <c r="F67" s="1">
+        <v>64</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2774,8 +2819,8 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G4:G66">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Yes">
+  <conditionalFormatting sqref="G4:G67">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2800,27 +2845,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdPermissions xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
-    <MigrationWizIdSecurityGroups xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
-    <MigrationWizId xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
-    <MigrationWizIdDocumentLibraryPermissions xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
-    <MigrationWizIdPermissionLevels xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005D604E489A710F48B80761E832F2A9CD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d18e01e9068d8b9ee0d6a8aa21ccc7c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c89f0296-b569-4583-a4b2-8889234c0295" xmlns:ns4="d7e6c0fb-87c1-48f5-8457-4cc066e411c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="56579f18c548d5b52f0079854658d5b1" ns3:_="" ns4:_="">
     <xsd:import namespace="c89f0296-b569-4583-a4b2-8889234c0295"/>
@@ -3061,10 +3085,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdPermissions xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
+    <MigrationWizIdSecurityGroups xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
+    <MigrationWizId xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
+    <MigrationWizIdDocumentLibraryPermissions xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
+    <MigrationWizIdPermissionLevels xmlns="c89f0296-b569-4583-a4b2-8889234c0295" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91BF9293-7B60-4F83-9196-3CF7B73475CD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1216411-492F-4F66-9460-0CE09A514303}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c89f0296-b569-4583-a4b2-8889234c0295"/>
+    <ds:schemaRef ds:uri="d7e6c0fb-87c1-48f5-8457-4cc066e411c5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3087,20 +3143,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1216411-492F-4F66-9460-0CE09A514303}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91BF9293-7B60-4F83-9196-3CF7B73475CD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c89f0296-b569-4583-a4b2-8889234c0295"/>
-    <ds:schemaRef ds:uri="d7e6c0fb-87c1-48f5-8457-4cc066e411c5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>